<commit_message>
replace output naming with shorter names
</commit_message>
<xml_diff>
--- a/outputs/03-estimate_cfr.xlsx
+++ b/outputs/03-estimate_cfr.xlsx
@@ -382,7 +382,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>without delay correction</t>
+          <t>naive</t>
         </is>
       </c>
       <c r="B2">
@@ -398,7 +398,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>with delay correction</t>
+          <t>corrected</t>
         </is>
       </c>
       <c r="B3">

</xml_diff>